<commit_message>
Corregir clave en modelo abarth
</commit_message>
<xml_diff>
--- a/xlsx/models.xlsx
+++ b/xlsx/models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\buscador-llantas.com\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5946A9E2-E52D-4305-B997-7F942A7112ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFB1AF3-8E87-41B6-8CD5-1A7885CBA460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{84D3D048-D589-4A4B-8B28-219B0DC07983}"/>
+    <workbookView xWindow="2565" yWindow="420" windowWidth="22395" windowHeight="11055" xr2:uid="{84D3D048-D589-4A4B-8B28-219B0DC07983}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$D$622</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2853,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AA45D9-D006-4460-9464-E14D7459B788}">
   <dimension ref="A1:D622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="C338" sqref="C338"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3348,9 +3351,8 @@
       <c r="A33" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B33" s="1" t="e">
-        <f>VLOOKUP(A33,[1]brands!$A$1:$B$53,2,1)</f>
-        <v>#N/A</v>
+      <c r="B33" s="1">
+        <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>377</v>
@@ -12195,6 +12197,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D622" xr:uid="{0E9095F2-E819-4E76-A3E0-EF75F12A98C5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C622">
     <sortCondition ref="C2:C622"/>
   </sortState>

</xml_diff>